<commit_message>
Medieval Overhaul Patches 번역 갱신
</commit_message>
<xml_diff>
--- a/Data/Medieval Overhaul Patches - 3015529451/Medieval Overhaul Patches - 3015529451.xlsx
+++ b/Data/Medieval Overhaul Patches - 3015529451/Medieval Overhaul Patches - 3015529451.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SteamLibrary\steamapps\common\RimWorld\Mods\MOD KOREAN TRANSLATE\1.4\Medieval Overhaul Patches - 3015529451\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDAB49A-F3F6-4A8A-8C85-826CCAE85D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E963E00-87F5-4CE1-8268-29FA8035930C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1550" uniqueCount="1124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1554" uniqueCount="1127">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -3058,25 +3058,7 @@
     <t>스펠트는 기원전 5000년경부터 재배되어 온 밀의 한 종류입니다. 식이섬유, 단백질(일반 밀보다 더 많이 함유되어 있음), 비타민과 미네랄의 좋은 공급원입니다. 스펠트는 결실을 맺기까지 거의 모든 재배 시즌이 걸립니다. 연약하고 시간이 많이 걸리지만, 이 곡식은 살짝만 만져도 밀가루로 부드럽게 부서지도록 유전자 조작을 거쳤습니다.</t>
   </si>
   <si>
-    <t>끈적거리는 초록색 줄기에서 나는 종잇장 같은 껍질 안에 둥글납작하고 향기로운 뿌리입니다. 양파는 쓸모가 많은 재료로, 채소 요리의 기본이 될 뿐만 아니라 고기 요리에도 맛있는 반찬입니다.\n\n&lt;color=#E5E54C&gt;게임 플레이 효과:&lt;/color&gt; 양파는 병충해에 영향을 받지 않습니다.</t>
-  </si>
-  <si>
     <t>얇은 초록색 덩굴에 자라는 특징적으로 거대한 오렌지색 야채로, 큰 것은 조금만 생긴다"는 것을 잘 보여줍니다. 그 자체로는 별로 맛있진 않지만</t>
-  </si>
-  <si>
-    <t>초록색 양배추로, 이파리가 켜켜이 쌓여 만들어진 식물입니다. 샐러드와 수프에 특히 좋은 재료입니다.\n\n&lt;color=#E5E54C&gt;게임 플레이 효과:&lt;/color&gt; 양배추는 독성 낙진에 영향을 받지 않으며 다른 식물과 달리 낙진으로 인해 죽지 않습니다.</t>
-  </si>
-  <si>
-    <t>이파리 많은 초록색 줄기 밑어는 나누어진 황백색의 구근이 달려 있습니다. 마늘은 다양한 음식에 좋은 양념이자 재료로 쓰이며, 다져서 볶은 후 재료로 쓰기도 하며, 가루내어 양념으로 쓰기도 합니다.\n\n&lt;color=#E5E54C&gt;게임 플레이 효과:&lt;/color&gt; 마늘은 수확량이 매우 적지만 거의 모든 지형에서 자랄 수 있으며 말린 마늘도 요리에 사용할 수 있기 때문에 썩는 데 시간이 많이 걸립니다.</t>
-  </si>
-  <si>
-    <t>덤불처럼 짧은 줄기에 달린 밝은 오렌지색 덩이줄기입니다. 그 자체로는 맛있는 간식은 아니지만 건강에 좋고, 삶거나 스튜에 넣거나 볶았을 때 어떤 음식에 넣어도 좋습니다.\n\n&lt;color=#E5E54C&gt;게임 플레이 효과:&lt;/color&gt; 같이 심기: 같은 맵에서 녹두를 재배하면 당근이 더 빨리 자랍니다(100개가 있는 경우 최대 30% 더 빨리 자랍니다).</t>
-  </si>
-  <si>
-    <t>빵, 음료, 스튜 및 기타 요리에 사용할 수 있는 곡물입니다. 통곡물인 보리는 식이섬유, 비타민, 미네랄을 제공합니다.\n\n&lt;color=#E5E54C&gt;게임 플레이 효과:&lt;/color&gt; 보리는 보리와 건초를 모두 생산한다는 의미에서 '이중 작물'입니다.</t>
-  </si>
-  <si>
-    <t>오트는 귀리라고도 불리며 씨앗을 위해 재배되는 이삭 곡물의 일종으로, 귀리는 요리에서 다양한 용도로 사용되며 식물성 우유로 만들 수도 있습니다.\n\n&lt;color=#E5E54C&gt;게임 플레이 효과:&lt;/color&gt; 귀리는 수확량은 낮지만 가루로 만들어 밀가루로 사용하거나 채소로 사용하거나 우유로 만들 수 있다는 점에서 매우 다재다능한 곡물입니다.</t>
   </si>
   <si>
     <t>식물성 우유 압착기</t>
@@ -3408,6 +3390,34 @@
   </si>
   <si>
     <t>VR_MO_Patch.settings.18.buttons.0.label</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>끈적거리는 초록색 줄기에서 나는 종잇장 같은 껍질 안에 둥글납작하고 향기로운 뿌리입니다. 양파는 쓸모가 많은 재료로, 채소 요리의 기본이 될 뿐만 아니라 고기 요리에도 맛있는 반찬입니다.\n\n&amp;lt;color=#E5E54C&gt;게임 플레이 효과:&amp;lt;/color&gt; 양파는 병충해에 영향을 받지 않습니다.</t>
+  </si>
+  <si>
+    <t>초록색 양배추로, 이파리가 켜켜이 쌓여 만들어진 식물입니다. 샐러드와 수프에 특히 좋은 재료입니다.\n\n&amp;lt;color=#E5E54C&gt;게임 플레이 효과:&amp;lt;/color&gt; 양배추는 독성 낙진에 영향을 받지 않으며 다른 식물과 달리 낙진으로 인해 죽지 않습니다.</t>
+  </si>
+  <si>
+    <t>이파리 많은 초록색 줄기 밑어는 나누어진 황백색의 구근이 달려 있습니다. 마늘은 다양한 음식에 좋은 양념이자 재료로 쓰이며, 다져서 볶은 후 재료로 쓰기도 하며, 가루내어 양념으로 쓰기도 합니다.\n\n&amp;lt;color=#E5E54C&gt;게임 플레이 효과:&amp;lt;/color&gt; 마늘은 수확량이 매우 적지만 거의 모든 지형에서 자랄 수 있으며 말린 마늘도 요리에 사용할 수 있기 때문에 썩는 데 시간이 많이 걸립니다.</t>
+  </si>
+  <si>
+    <t>덤불처럼 짧은 줄기에 달린 밝은 오렌지색 덩이줄기입니다. 그 자체로는 맛있는 간식은 아니지만 건강에 좋고, 삶거나 스튜에 넣거나 볶았을 때 어떤 음식에 넣어도 좋습니다.\n\n&amp;lt;color=#E5E54C&gt;게임 플레이 효과:&amp;lt;/color&gt; 같이 심기: 같은 맵에서 녹두를 재배하면 당근이 더 빨리 자랍니다(100개가 있는 경우 최대 30% 더 빨리 자랍니다).</t>
+  </si>
+  <si>
+    <t>빵, 음료, 스튜 및 기타 요리에 사용할 수 있는 곡물입니다. 통곡물인 보리는 식이섬유, 비타민, 미네랄을 제공합니다.\n\n&amp;lt;color=#E5E54C&gt;게임 플레이 효과:&amp;lt;/color&gt; 보리는 보리와 건초를 모두 생산한다는 의미에서 '이중 작물'입니다.</t>
+  </si>
+  <si>
+    <t>오트는 귀리라고도 불리며 씨앗을 위해 재배되는 이삭 곡물의 일종으로, 귀리는 요리에서 다양한 용도로 사용되며 식물성 우유로 만들 수도 있습니다.\n\n&amp;lt;color=#E5E54C&gt;게임 플레이 효과:&amp;lt;/color&gt; 귀리는 수확량은 낮지만 가루로 만들어 밀가루로 사용하거나 채소로 사용하거나 우유로 만들 수 있다는 점에서 매우 다재다능한 곡물입니다.</t>
+  </si>
+  <si>
+    <t>DankPyon_GenericHides.label</t>
+  </si>
+  <si>
+    <t>generic hides</t>
+  </si>
+  <si>
+    <t>일반 가죽</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3782,10 +3792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F386"/>
+  <dimension ref="A1:F387"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A353" workbookViewId="0">
-      <selection activeCell="C379" sqref="C379"/>
+    <sheetView tabSelected="1" topLeftCell="A367" workbookViewId="0">
+      <selection activeCell="E388" sqref="E388"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -7786,7 +7796,7 @@
       </c>
       <c r="D265" s="1"/>
       <c r="E265" s="5" t="s">
-        <v>1007</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.3">
@@ -7801,7 +7811,7 @@
       </c>
       <c r="D266" s="1"/>
       <c r="E266" s="5" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.3">
@@ -7816,7 +7826,7 @@
       </c>
       <c r="D267" s="1"/>
       <c r="E267" s="5" t="s">
-        <v>1009</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.3">
@@ -7831,7 +7841,7 @@
       </c>
       <c r="D268" s="1"/>
       <c r="E268" s="5" t="s">
-        <v>1010</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.3">
@@ -7846,7 +7856,7 @@
       </c>
       <c r="D269" s="1"/>
       <c r="E269" s="5" t="s">
-        <v>1011</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.3">
@@ -7861,7 +7871,7 @@
       </c>
       <c r="D270" s="1"/>
       <c r="E270" s="5" t="s">
-        <v>1012</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.3">
@@ -7876,7 +7886,7 @@
       </c>
       <c r="D271" s="1"/>
       <c r="E271" s="5" t="s">
-        <v>1013</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.3">
@@ -7891,7 +7901,7 @@
       </c>
       <c r="D272" s="1"/>
       <c r="E272" s="5" t="s">
-        <v>1014</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.3">
@@ -7906,7 +7916,7 @@
       </c>
       <c r="D273" s="1"/>
       <c r="E273" s="5" t="s">
-        <v>1015</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.3">
@@ -7921,7 +7931,7 @@
       </c>
       <c r="D274" s="1"/>
       <c r="E274" s="5" t="s">
-        <v>1016</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.3">
@@ -7936,7 +7946,7 @@
       </c>
       <c r="D275" s="1"/>
       <c r="E275" s="5" t="s">
-        <v>1017</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.3">
@@ -7951,7 +7961,7 @@
       </c>
       <c r="D276" s="1"/>
       <c r="E276" s="5" t="s">
-        <v>1018</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.3">
@@ -7966,7 +7976,7 @@
       </c>
       <c r="D277" s="1"/>
       <c r="E277" s="5" t="s">
-        <v>1019</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.3">
@@ -7981,7 +7991,7 @@
       </c>
       <c r="D278" s="1"/>
       <c r="E278" s="5" t="s">
-        <v>1020</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.3">
@@ -7996,7 +8006,7 @@
       </c>
       <c r="D279" s="1"/>
       <c r="E279" s="5" t="s">
-        <v>1021</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.3">
@@ -8011,7 +8021,7 @@
       </c>
       <c r="D280" s="1"/>
       <c r="E280" s="5" t="s">
-        <v>1022</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.3">
@@ -8026,7 +8036,7 @@
       </c>
       <c r="D281" s="1"/>
       <c r="E281" s="5" t="s">
-        <v>1023</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.3">
@@ -8041,7 +8051,7 @@
       </c>
       <c r="D282" s="1"/>
       <c r="E282" s="5" t="s">
-        <v>1024</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.3">
@@ -8056,7 +8066,7 @@
       </c>
       <c r="D283" s="1"/>
       <c r="E283" s="5" t="s">
-        <v>1025</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.3">
@@ -8071,7 +8081,7 @@
       </c>
       <c r="D284" s="1"/>
       <c r="E284" s="5" t="s">
-        <v>1026</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.3">
@@ -8086,7 +8096,7 @@
       </c>
       <c r="D285" s="1"/>
       <c r="E285" s="5" t="s">
-        <v>1027</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.3">
@@ -8101,7 +8111,7 @@
       </c>
       <c r="D286" s="1"/>
       <c r="E286" s="5" t="s">
-        <v>1028</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.3">
@@ -8116,7 +8126,7 @@
       </c>
       <c r="D287" s="1"/>
       <c r="E287" s="5" t="s">
-        <v>1029</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.3">
@@ -8131,7 +8141,7 @@
       </c>
       <c r="D288" s="1"/>
       <c r="E288" s="5" t="s">
-        <v>1030</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.3">
@@ -8146,7 +8156,7 @@
       </c>
       <c r="D289" s="1"/>
       <c r="E289" s="5" t="s">
-        <v>1031</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.3">
@@ -8161,7 +8171,7 @@
       </c>
       <c r="D290" s="1"/>
       <c r="E290" s="5" t="s">
-        <v>1032</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.3">
@@ -8176,7 +8186,7 @@
       </c>
       <c r="D291" s="1"/>
       <c r="E291" s="5" t="s">
-        <v>1033</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.3">
@@ -8191,7 +8201,7 @@
       </c>
       <c r="D292" s="1"/>
       <c r="E292" s="5" t="s">
-        <v>1034</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.3">
@@ -8206,7 +8216,7 @@
       </c>
       <c r="D293" s="1"/>
       <c r="E293" s="5" t="s">
-        <v>1035</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.3">
@@ -8221,7 +8231,7 @@
       </c>
       <c r="D294" s="1"/>
       <c r="E294" s="5" t="s">
-        <v>1036</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.3">
@@ -8236,7 +8246,7 @@
       </c>
       <c r="D295" s="1"/>
       <c r="E295" s="5" t="s">
-        <v>1037</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.3">
@@ -8251,7 +8261,7 @@
       </c>
       <c r="D296" s="1"/>
       <c r="E296" s="5" t="s">
-        <v>1038</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.3">
@@ -8266,7 +8276,7 @@
       </c>
       <c r="D297" s="1"/>
       <c r="E297" s="5" t="s">
-        <v>1039</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.3">
@@ -8281,7 +8291,7 @@
       </c>
       <c r="D298" s="1"/>
       <c r="E298" s="5" t="s">
-        <v>1040</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.3">
@@ -8296,7 +8306,7 @@
       </c>
       <c r="D299" s="1"/>
       <c r="E299" s="5" t="s">
-        <v>1041</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.3">
@@ -8311,7 +8321,7 @@
       </c>
       <c r="D300" s="1"/>
       <c r="E300" s="5" t="s">
-        <v>1042</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.3">
@@ -8326,7 +8336,7 @@
       </c>
       <c r="D301" s="1"/>
       <c r="E301" s="5" t="s">
-        <v>1043</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.3">
@@ -8341,7 +8351,7 @@
       </c>
       <c r="D302" s="1"/>
       <c r="E302" s="5" t="s">
-        <v>1044</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.3">
@@ -8356,7 +8366,7 @@
       </c>
       <c r="D303" s="1"/>
       <c r="E303" s="5" t="s">
-        <v>1045</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.3">
@@ -8371,7 +8381,7 @@
       </c>
       <c r="D304" s="1"/>
       <c r="E304" s="5" t="s">
-        <v>1046</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.3">
@@ -8386,7 +8396,7 @@
       </c>
       <c r="D305" s="1"/>
       <c r="E305" s="5" t="s">
-        <v>1045</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.3">
@@ -8401,7 +8411,7 @@
       </c>
       <c r="D306" s="1"/>
       <c r="E306" s="5" t="s">
-        <v>1047</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.3">
@@ -8416,7 +8426,7 @@
       </c>
       <c r="D307" s="1"/>
       <c r="E307" s="5" t="s">
-        <v>1048</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.3">
@@ -8431,7 +8441,7 @@
       </c>
       <c r="D308" s="1"/>
       <c r="E308" s="5" t="s">
-        <v>1049</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.3">
@@ -8446,7 +8456,7 @@
       </c>
       <c r="D309" s="1"/>
       <c r="E309" s="5" t="s">
-        <v>1048</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.3">
@@ -8461,7 +8471,7 @@
       </c>
       <c r="D310" s="1"/>
       <c r="E310" s="5" t="s">
-        <v>1047</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.3">
@@ -8476,7 +8486,7 @@
       </c>
       <c r="D311" s="1"/>
       <c r="E311" s="5" t="s">
-        <v>1050</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.3">
@@ -8491,7 +8501,7 @@
       </c>
       <c r="D312" s="1"/>
       <c r="E312" s="5" t="s">
-        <v>1051</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.3">
@@ -8506,7 +8516,7 @@
       </c>
       <c r="D313" s="1"/>
       <c r="E313" s="5" t="s">
-        <v>1050</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.3">
@@ -8521,7 +8531,7 @@
       </c>
       <c r="D314" s="1"/>
       <c r="E314" s="5" t="s">
-        <v>1047</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.3">
@@ -8536,7 +8546,7 @@
       </c>
       <c r="D315" s="1"/>
       <c r="E315" s="5" t="s">
-        <v>1052</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.3">
@@ -8551,7 +8561,7 @@
       </c>
       <c r="D316" s="1"/>
       <c r="E316" s="5" t="s">
-        <v>1053</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.3">
@@ -8566,7 +8576,7 @@
       </c>
       <c r="D317" s="1"/>
       <c r="E317" s="5" t="s">
-        <v>1054</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.3">
@@ -8581,7 +8591,7 @@
       </c>
       <c r="D318" s="1"/>
       <c r="E318" s="5" t="s">
-        <v>1055</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="319" spans="1:5" x14ac:dyDescent="0.3">
@@ -8596,7 +8606,7 @@
       </c>
       <c r="D319" s="1"/>
       <c r="E319" s="5" t="s">
-        <v>1056</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.3">
@@ -8611,7 +8621,7 @@
       </c>
       <c r="D320" s="1"/>
       <c r="E320" s="5" t="s">
-        <v>1057</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.3">
@@ -8626,7 +8636,7 @@
       </c>
       <c r="D321" s="1"/>
       <c r="E321" s="5" t="s">
-        <v>1058</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.3">
@@ -8641,7 +8651,7 @@
       </c>
       <c r="D322" s="1"/>
       <c r="E322" s="5" t="s">
-        <v>1059</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.3">
@@ -8656,7 +8666,7 @@
       </c>
       <c r="D323" s="1"/>
       <c r="E323" s="5" t="s">
-        <v>1060</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="324" spans="1:5" x14ac:dyDescent="0.3">
@@ -8671,7 +8681,7 @@
       </c>
       <c r="D324" s="1"/>
       <c r="E324" s="5" t="s">
-        <v>1061</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="325" spans="1:5" x14ac:dyDescent="0.3">
@@ -8686,7 +8696,7 @@
       </c>
       <c r="D325" s="1"/>
       <c r="E325" s="5" t="s">
-        <v>1062</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.3">
@@ -8701,7 +8711,7 @@
       </c>
       <c r="D326" s="1"/>
       <c r="E326" s="5" t="s">
-        <v>1063</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.3">
@@ -8716,7 +8726,7 @@
       </c>
       <c r="D327" s="1"/>
       <c r="E327" s="5" t="s">
-        <v>1064</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="328" spans="1:5" x14ac:dyDescent="0.3">
@@ -8731,7 +8741,7 @@
       </c>
       <c r="D328" s="1"/>
       <c r="E328" s="5" t="s">
-        <v>1065</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.3">
@@ -8746,7 +8756,7 @@
       </c>
       <c r="D329" s="1"/>
       <c r="E329" s="5" t="s">
-        <v>1066</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="330" spans="1:5" x14ac:dyDescent="0.3">
@@ -8761,7 +8771,7 @@
       </c>
       <c r="D330" s="1"/>
       <c r="E330" s="5" t="s">
-        <v>1067</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="331" spans="1:5" x14ac:dyDescent="0.3">
@@ -8776,7 +8786,7 @@
       </c>
       <c r="D331" s="1"/>
       <c r="E331" s="5" t="s">
-        <v>1068</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.3">
@@ -8791,7 +8801,7 @@
       </c>
       <c r="D332" s="1"/>
       <c r="E332" s="5" t="s">
-        <v>1069</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.3">
@@ -8806,7 +8816,7 @@
       </c>
       <c r="D333" s="1"/>
       <c r="E333" s="5" t="s">
-        <v>1070</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.3">
@@ -8821,7 +8831,7 @@
       </c>
       <c r="D334" s="1"/>
       <c r="E334" s="5" t="s">
-        <v>1071</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.3">
@@ -8836,7 +8846,7 @@
       </c>
       <c r="D335" s="1"/>
       <c r="E335" s="5" t="s">
-        <v>1072</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="336" spans="1:5" x14ac:dyDescent="0.3">
@@ -8851,7 +8861,7 @@
       </c>
       <c r="D336" s="1"/>
       <c r="E336" s="5" t="s">
-        <v>1073</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.3">
@@ -8866,7 +8876,7 @@
       </c>
       <c r="D337" s="1"/>
       <c r="E337" s="5" t="s">
-        <v>1074</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.3">
@@ -8881,7 +8891,7 @@
       </c>
       <c r="D338" s="1"/>
       <c r="E338" s="5" t="s">
-        <v>1075</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="339" spans="1:5" x14ac:dyDescent="0.3">
@@ -8896,7 +8906,7 @@
       </c>
       <c r="D339" s="1"/>
       <c r="E339" s="5" t="s">
-        <v>1076</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="340" spans="1:5" x14ac:dyDescent="0.3">
@@ -8911,7 +8921,7 @@
       </c>
       <c r="D340" s="1"/>
       <c r="E340" s="5" t="s">
-        <v>1077</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="341" spans="1:5" x14ac:dyDescent="0.3">
@@ -8926,7 +8936,7 @@
       </c>
       <c r="D341" s="1"/>
       <c r="E341" s="5" t="s">
-        <v>1078</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="342" spans="1:5" x14ac:dyDescent="0.3">
@@ -8941,7 +8951,7 @@
       </c>
       <c r="D342" s="1"/>
       <c r="E342" s="5" t="s">
-        <v>1079</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="343" spans="1:5" x14ac:dyDescent="0.3">
@@ -8956,7 +8966,7 @@
       </c>
       <c r="D343" s="1"/>
       <c r="E343" s="5" t="s">
-        <v>1080</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="344" spans="1:5" x14ac:dyDescent="0.3">
@@ -8971,7 +8981,7 @@
       </c>
       <c r="D344" s="1"/>
       <c r="E344" s="5" t="s">
-        <v>1081</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="345" spans="1:5" x14ac:dyDescent="0.3">
@@ -8986,7 +8996,7 @@
       </c>
       <c r="D345" s="1"/>
       <c r="E345" s="5" t="s">
-        <v>1082</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.3">
@@ -9001,7 +9011,7 @@
       </c>
       <c r="D346" s="1"/>
       <c r="E346" s="5" t="s">
-        <v>1083</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="347" spans="1:5" x14ac:dyDescent="0.3">
@@ -9016,7 +9026,7 @@
       </c>
       <c r="D347" s="1"/>
       <c r="E347" s="5" t="s">
-        <v>1084</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="348" spans="1:5" x14ac:dyDescent="0.3">
@@ -9031,7 +9041,7 @@
       </c>
       <c r="D348" s="1"/>
       <c r="E348" s="5" t="s">
-        <v>1085</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.3">
@@ -9046,7 +9056,7 @@
       </c>
       <c r="D349" s="1"/>
       <c r="E349" s="5" t="s">
-        <v>1086</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.3">
@@ -9061,7 +9071,7 @@
       </c>
       <c r="D350" s="1"/>
       <c r="E350" s="5" t="s">
-        <v>1087</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.3">
@@ -9076,7 +9086,7 @@
       </c>
       <c r="D351" s="1"/>
       <c r="E351" s="5" t="s">
-        <v>1088</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="352" spans="1:5" x14ac:dyDescent="0.3">
@@ -9091,7 +9101,7 @@
       </c>
       <c r="D352" s="1"/>
       <c r="E352" s="5" t="s">
-        <v>1089</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="353" spans="1:5" x14ac:dyDescent="0.3">
@@ -9106,7 +9116,7 @@
       </c>
       <c r="D353" s="1"/>
       <c r="E353" s="5" t="s">
-        <v>1090</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="354" spans="1:5" x14ac:dyDescent="0.3">
@@ -9121,7 +9131,7 @@
       </c>
       <c r="D354" s="1"/>
       <c r="E354" s="5" t="s">
-        <v>1091</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="355" spans="1:5" x14ac:dyDescent="0.3">
@@ -9136,7 +9146,7 @@
       </c>
       <c r="D355" s="1"/>
       <c r="E355" s="5" t="s">
-        <v>1092</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="356" spans="1:5" x14ac:dyDescent="0.3">
@@ -9151,7 +9161,7 @@
       </c>
       <c r="D356" s="1"/>
       <c r="E356" s="5" t="s">
-        <v>1092</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="357" spans="1:5" x14ac:dyDescent="0.3">
@@ -9166,7 +9176,7 @@
       </c>
       <c r="D357" s="1"/>
       <c r="E357" s="5" t="s">
-        <v>1093</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="358" spans="1:5" x14ac:dyDescent="0.3">
@@ -9181,7 +9191,7 @@
       </c>
       <c r="D358" s="1"/>
       <c r="E358" s="5" t="s">
-        <v>1094</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="359" spans="1:5" x14ac:dyDescent="0.3">
@@ -9196,7 +9206,7 @@
       </c>
       <c r="D359" s="1"/>
       <c r="E359" s="5" t="s">
-        <v>1094</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="360" spans="1:5" x14ac:dyDescent="0.3">
@@ -9211,7 +9221,7 @@
       </c>
       <c r="D360" s="1"/>
       <c r="E360" s="5" t="s">
-        <v>1095</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="361" spans="1:5" x14ac:dyDescent="0.3">
@@ -9226,7 +9236,7 @@
       </c>
       <c r="D361" s="1"/>
       <c r="E361" s="5" t="s">
-        <v>1096</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="362" spans="1:5" x14ac:dyDescent="0.3">
@@ -9241,7 +9251,7 @@
       </c>
       <c r="D362" s="1"/>
       <c r="E362" s="5" t="s">
-        <v>1097</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="363" spans="1:5" x14ac:dyDescent="0.3">
@@ -9256,7 +9266,7 @@
       </c>
       <c r="D363" s="1"/>
       <c r="E363" s="5" t="s">
-        <v>1098</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.3">
@@ -9271,7 +9281,7 @@
       </c>
       <c r="D364" s="1"/>
       <c r="E364" s="5" t="s">
-        <v>1099</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="365" spans="1:5" x14ac:dyDescent="0.3">
@@ -9286,7 +9296,7 @@
       </c>
       <c r="D365" s="1"/>
       <c r="E365" s="5" t="s">
-        <v>1100</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="366" spans="1:5" x14ac:dyDescent="0.3">
@@ -9301,7 +9311,7 @@
       </c>
       <c r="D366" s="1"/>
       <c r="E366" s="5" t="s">
-        <v>1101</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="367" spans="1:5" x14ac:dyDescent="0.3">
@@ -9316,7 +9326,7 @@
       </c>
       <c r="D367" s="1"/>
       <c r="E367" s="5" t="s">
-        <v>1102</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="368" spans="1:5" x14ac:dyDescent="0.3">
@@ -9331,7 +9341,7 @@
       </c>
       <c r="D368" s="1"/>
       <c r="E368" s="5" t="s">
-        <v>1103</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="369" spans="1:5" x14ac:dyDescent="0.3">
@@ -9346,7 +9356,7 @@
       </c>
       <c r="D369" s="1"/>
       <c r="E369" s="5" t="s">
-        <v>1104</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="370" spans="1:5" x14ac:dyDescent="0.3">
@@ -9361,7 +9371,7 @@
       </c>
       <c r="D370" s="1"/>
       <c r="E370" s="5" t="s">
-        <v>1105</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="371" spans="1:5" x14ac:dyDescent="0.3">
@@ -9376,7 +9386,7 @@
       </c>
       <c r="D371" s="1"/>
       <c r="E371" s="5" t="s">
-        <v>1106</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="372" spans="1:5" x14ac:dyDescent="0.3">
@@ -9391,7 +9401,7 @@
       </c>
       <c r="D372" s="1"/>
       <c r="E372" s="5" t="s">
-        <v>1107</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="373" spans="1:5" x14ac:dyDescent="0.3">
@@ -9406,7 +9416,7 @@
       </c>
       <c r="D373" s="1"/>
       <c r="E373" s="5" t="s">
-        <v>1108</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="374" spans="1:5" x14ac:dyDescent="0.3">
@@ -9421,7 +9431,7 @@
       </c>
       <c r="D374" s="1"/>
       <c r="E374" s="5" t="s">
-        <v>1109</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="375" spans="1:5" x14ac:dyDescent="0.3">
@@ -9436,7 +9446,7 @@
       </c>
       <c r="D375" s="1"/>
       <c r="E375" s="5" t="s">
-        <v>1110</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="376" spans="1:5" x14ac:dyDescent="0.3">
@@ -9451,7 +9461,7 @@
       </c>
       <c r="D376" s="1"/>
       <c r="E376" s="5" t="s">
-        <v>1111</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="377" spans="1:5" x14ac:dyDescent="0.3">
@@ -9466,7 +9476,7 @@
       </c>
       <c r="D377" s="1"/>
       <c r="E377" s="5" t="s">
-        <v>1112</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="378" spans="1:5" x14ac:dyDescent="0.3">
@@ -9481,7 +9491,7 @@
       </c>
       <c r="D378" s="1"/>
       <c r="E378" s="5" t="s">
-        <v>1113</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="379" spans="1:5" x14ac:dyDescent="0.3">
@@ -9492,10 +9502,10 @@
         <v>6</v>
       </c>
       <c r="C379" t="s">
-        <v>1123</v>
+        <v>1117</v>
       </c>
       <c r="E379" s="5" t="s">
-        <v>1114</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="380" spans="1:5" x14ac:dyDescent="0.3">
@@ -9509,7 +9519,7 @@
         <v>771</v>
       </c>
       <c r="E380" s="5" t="s">
-        <v>1115</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="381" spans="1:5" x14ac:dyDescent="0.3">
@@ -9523,7 +9533,7 @@
         <v>37</v>
       </c>
       <c r="E381" s="5" t="s">
-        <v>1116</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="382" spans="1:5" x14ac:dyDescent="0.3">
@@ -9537,7 +9547,7 @@
         <v>772</v>
       </c>
       <c r="E382" s="5" t="s">
-        <v>1117</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="383" spans="1:5" x14ac:dyDescent="0.3">
@@ -9548,10 +9558,10 @@
         <v>6</v>
       </c>
       <c r="C383" t="s">
-        <v>1122</v>
+        <v>1116</v>
       </c>
       <c r="E383" s="5" t="s">
-        <v>1118</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="384" spans="1:5" x14ac:dyDescent="0.3">
@@ -9565,7 +9575,7 @@
         <v>773</v>
       </c>
       <c r="E384" s="5" t="s">
-        <v>1119</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="385" spans="1:5" x14ac:dyDescent="0.3">
@@ -9579,7 +9589,7 @@
         <v>774</v>
       </c>
       <c r="E385" s="5" t="s">
-        <v>1120</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="386" spans="1:5" x14ac:dyDescent="0.3">
@@ -9593,7 +9603,21 @@
         <v>775</v>
       </c>
       <c r="E386" s="5" t="s">
-        <v>1121</v>
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="387" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B387" t="s">
+        <v>294</v>
+      </c>
+      <c r="C387" t="s">
+        <v>1124</v>
+      </c>
+      <c r="D387" t="s">
+        <v>1125</v>
+      </c>
+      <c r="E387" s="5" t="s">
+        <v>1126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Medieval Overhaul Patches - 3015529451 번역 갱신
</commit_message>
<xml_diff>
--- a/Data/Medieval Overhaul Patches - 3015529451/Medieval Overhaul Patches - 3015529451.xlsx
+++ b/Data/Medieval Overhaul Patches - 3015529451/Medieval Overhaul Patches - 3015529451.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SteamLibrary\steamapps\common\RimWorld\Mods\MOD KOREAN TRANSLATE\1.4\Medieval Overhaul Patches - 3015529451\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E963E00-87F5-4CE1-8268-29FA8035930C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB0714C-92CD-4546-B933-5C759C11B6CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1554" uniqueCount="1127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1599" uniqueCount="1161">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -3419,6 +3419,109 @@
   <si>
     <t>일반 가죽</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SettingsMenuDef: VR_MO_Patch.settings.16.label 'Alchemy Table Drugs?'</t>
+  </si>
+  <si>
+    <t>SettingsMenuDef: VR_MO_Patch.settings.16.tooltip 'Allows the alchemy table to inherit drug recipes.'</t>
+  </si>
+  <si>
+    <t>SettingsMenuDef: VR_MO_Patch.settings.18.text 'Trimmed Meat Options:'</t>
+  </si>
+  <si>
+    <t>SettingsMenuDef: VR_MO_Patch.settings.19.buttons.0.tooltip 'No trimmed meat.'</t>
+  </si>
+  <si>
+    <t>SettingsMenuDef: VR_MO_Patch.settings.19.buttons.1.label 'MO Trimmed Meat Recipe:'</t>
+  </si>
+  <si>
+    <t>SettingsMenuDef: VR_MO_Patch.settings.19.buttons.1.tooltip 'This enables a trimmed meat recipe for the extra verisimilitude.'</t>
+  </si>
+  <si>
+    <t>SettingsMenuDef: VR_MO_Patch.settings.22.tooltip 'Adds various Medieval Overhaul plants to biomes as wild plants.'</t>
+  </si>
+  <si>
+    <t>SettingsMenuDef: VR_MO_Patch.settings.23.label 'Reset Settings'</t>
+  </si>
+  <si>
+    <t>SettingsMenuDef: VR_MO_Patch.settings.23.message 'Are you sure?'</t>
+  </si>
+  <si>
+    <t>VR_MO_Patch.settings.16.label</t>
+  </si>
+  <si>
+    <t>VR_MO_Patch.settings.16.tooltip</t>
+  </si>
+  <si>
+    <t>VR_MO_Patch.settings.18.text</t>
+  </si>
+  <si>
+    <t>VR_MO_Patch.settings.19.buttons.0.tooltip</t>
+  </si>
+  <si>
+    <t>VR_MO_Patch.settings.19.buttons.1.label</t>
+  </si>
+  <si>
+    <t>VR_MO_Patch.settings.19.buttons.1.tooltip</t>
+  </si>
+  <si>
+    <t>VR_MO_Patch.settings.22.tooltip</t>
+  </si>
+  <si>
+    <t>VR_MO_Patch.settings.23.label</t>
+  </si>
+  <si>
+    <t>VR_MO_Patch.settings.23.message</t>
+  </si>
+  <si>
+    <t>Alchemy Table Drugs?</t>
+  </si>
+  <si>
+    <t>Allows the alchemy table to inherit drug recipes.</t>
+  </si>
+  <si>
+    <t>Trimmed Meat Options:</t>
+  </si>
+  <si>
+    <t>No trimmed meat.</t>
+  </si>
+  <si>
+    <t>MO Trimmed Meat Recipe:</t>
+  </si>
+  <si>
+    <t>Adds various Medieval Overhaul plants to biomes as wild plants.</t>
+  </si>
+  <si>
+    <t>Reset Settings</t>
+  </si>
+  <si>
+    <t>Are you sure?</t>
+  </si>
+  <si>
+    <t>연금술 테이블이 약품 레시피를 상속할 수 있도록 허용합니다.</t>
+  </si>
+  <si>
+    <t>연금술 테이블 약?</t>
+  </si>
+  <si>
+    <t>손질된 고기 없음.</t>
+  </si>
+  <si>
+    <t>MO 손질된 고기 레시피:</t>
+  </si>
+  <si>
+    <t>This enables a trimmed meat recipe for the extra verisimilitude.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이렇게 하면 고기를 손질하여 더욱 사실적인 레시피를 만들 수 있습니다.</t>
+  </si>
+  <si>
+    <t>생물군에 다양한 Medieval Overhaul 식물을  야생 식물로 추가합니다.</t>
+  </si>
+  <si>
+    <t>확실하신가요?</t>
   </si>
 </sst>
 </file>
@@ -3792,10 +3895,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F387"/>
+  <dimension ref="A1:G396"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A367" workbookViewId="0">
-      <selection activeCell="E388" sqref="E388"/>
+      <selection activeCell="D392" sqref="D392"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -9578,7 +9681,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="385" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A385" s="5" t="s">
         <v>714</v>
       </c>
@@ -9592,7 +9695,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="386" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A386" s="5" t="s">
         <v>715</v>
       </c>
@@ -9606,7 +9709,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="387" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B387" t="s">
         <v>294</v>
       </c>
@@ -9618,6 +9721,195 @@
       </c>
       <c r="E387" s="5" t="s">
         <v>1126</v>
+      </c>
+    </row>
+    <row r="388" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B388" t="s">
+        <v>6</v>
+      </c>
+      <c r="C388" t="s">
+        <v>1136</v>
+      </c>
+      <c r="D388" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E388" t="s">
+        <v>1154</v>
+      </c>
+      <c r="F388" t="s">
+        <v>1127</v>
+      </c>
+      <c r="G388" t="str">
+        <f>MID(F388,FIND("'",F388)+1,FIND("'",F388,FIND("'",F388)+1)-FIND("'",F388)-1)</f>
+        <v>Alchemy Table Drugs?</v>
+      </c>
+    </row>
+    <row r="389" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B389" t="s">
+        <v>6</v>
+      </c>
+      <c r="C389" t="s">
+        <v>1137</v>
+      </c>
+      <c r="D389" t="s">
+        <v>1146</v>
+      </c>
+      <c r="E389" t="s">
+        <v>1153</v>
+      </c>
+      <c r="F389" t="s">
+        <v>1128</v>
+      </c>
+      <c r="G389" t="str">
+        <f t="shared" ref="G389:G396" si="0">MID(F389,FIND("'",F389)+1,FIND("'",F389,FIND("'",F389)+1)-FIND("'",F389)-1)</f>
+        <v>Allows the alchemy table to inherit drug recipes.</v>
+      </c>
+    </row>
+    <row r="390" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B390" t="s">
+        <v>6</v>
+      </c>
+      <c r="C390" t="s">
+        <v>1138</v>
+      </c>
+      <c r="D390" t="s">
+        <v>1147</v>
+      </c>
+      <c r="E390" t="s">
+        <v>1107</v>
+      </c>
+      <c r="F390" t="s">
+        <v>1129</v>
+      </c>
+      <c r="G390" t="str">
+        <f t="shared" si="0"/>
+        <v>Trimmed Meat Options:</v>
+      </c>
+    </row>
+    <row r="391" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B391" t="s">
+        <v>6</v>
+      </c>
+      <c r="C391" t="s">
+        <v>1139</v>
+      </c>
+      <c r="D391" t="s">
+        <v>1148</v>
+      </c>
+      <c r="E391" t="s">
+        <v>1155</v>
+      </c>
+      <c r="F391" t="s">
+        <v>1130</v>
+      </c>
+      <c r="G391" t="str">
+        <f t="shared" si="0"/>
+        <v>No trimmed meat.</v>
+      </c>
+    </row>
+    <row r="392" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B392" t="s">
+        <v>6</v>
+      </c>
+      <c r="C392" t="s">
+        <v>1140</v>
+      </c>
+      <c r="D392" t="s">
+        <v>1149</v>
+      </c>
+      <c r="E392" t="s">
+        <v>1156</v>
+      </c>
+      <c r="F392" t="s">
+        <v>1131</v>
+      </c>
+      <c r="G392" t="str">
+        <f t="shared" si="0"/>
+        <v>MO Trimmed Meat Recipe:</v>
+      </c>
+    </row>
+    <row r="393" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B393" t="s">
+        <v>6</v>
+      </c>
+      <c r="C393" t="s">
+        <v>1141</v>
+      </c>
+      <c r="D393" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E393" t="s">
+        <v>1158</v>
+      </c>
+      <c r="F393" t="s">
+        <v>1132</v>
+      </c>
+      <c r="G393" t="str">
+        <f t="shared" si="0"/>
+        <v>This enables a trimmed meat recipe for the extra verisimilitude.</v>
+      </c>
+    </row>
+    <row r="394" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B394" t="s">
+        <v>6</v>
+      </c>
+      <c r="C394" t="s">
+        <v>1142</v>
+      </c>
+      <c r="D394" t="s">
+        <v>1150</v>
+      </c>
+      <c r="E394" t="s">
+        <v>1159</v>
+      </c>
+      <c r="F394" t="s">
+        <v>1133</v>
+      </c>
+      <c r="G394" t="str">
+        <f t="shared" si="0"/>
+        <v>Adds various Medieval Overhaul plants to biomes as wild plants.</v>
+      </c>
+    </row>
+    <row r="395" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B395" t="s">
+        <v>6</v>
+      </c>
+      <c r="C395" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D395" t="s">
+        <v>1151</v>
+      </c>
+      <c r="E395" t="s">
+        <v>1114</v>
+      </c>
+      <c r="F395" t="s">
+        <v>1134</v>
+      </c>
+      <c r="G395" t="str">
+        <f t="shared" si="0"/>
+        <v>Reset Settings</v>
+      </c>
+    </row>
+    <row r="396" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B396" t="s">
+        <v>6</v>
+      </c>
+      <c r="C396" t="s">
+        <v>1144</v>
+      </c>
+      <c r="D396" t="s">
+        <v>1152</v>
+      </c>
+      <c r="E396" t="s">
+        <v>1160</v>
+      </c>
+      <c r="F396" t="s">
+        <v>1135</v>
+      </c>
+      <c r="G396" t="str">
+        <f t="shared" si="0"/>
+        <v>Are you sure?</v>
       </c>
     </row>
   </sheetData>

</xml_diff>